<commit_message>
add sysC; finished checking results against Trimmer et al.; minor bug fix; add system reports
</commit_message>
<xml_diff>
--- a/qsdsan/data/_impact_item.xlsx
+++ b/qsdsan/data/_impact_item.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/qs_yl/qsdsan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{935E0A0B-8DD3-6742-99D3-41177F9390EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C0E89C8A-0DCF-8443-8EC3-83112B8CAC8E}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="8_{935E0A0B-8DD3-6742-99D3-41177F9390EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2A4D037B-7307-C842-B5BB-8B02115339E4}"/>
   <bookViews>
     <workbookView xWindow="9380" yWindow="2260" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
@@ -632,7 +632,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -865,13 +865,16 @@
         <v>22</v>
       </c>
       <c r="C10" s="5">
-        <v>0.65</v>
+        <f>4.33+0.65</f>
+        <v>4.9800000000000004</v>
       </c>
       <c r="D10" s="5">
-        <v>0.57999999999999996</v>
+        <f>D9+0.58</f>
+        <v>3.65</v>
       </c>
       <c r="E10" s="5">
-        <v>0.71</v>
+        <f>E9+0.71</f>
+        <v>6.21</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>1</v>

</xml_diff>